<commit_message>
deleted chinese in data
</commit_message>
<xml_diff>
--- a/data/authorData.xlsx
+++ b/data/authorData.xlsx
@@ -1,53 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1f6cda4feb914768/Desktop/CS225/finalProject/datagrab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laskyj/Study/UIUC/2022 Fall/CS225/BiliGraph/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B288B7CE-FFCD-4E43-AF05-1895DA22718E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C94EC3-051B-D94A-B939-BE1783D4234E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30000" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="authorData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>UID</t>
-  </si>
-  <si>
-    <t>Nick Name</t>
   </si>
   <si>
     <t>Average View</t>
@@ -58,325 +46,16 @@
   <si>
     <t>Average Coin</t>
   </si>
-  <si>
-    <t>布锅锅</t>
-  </si>
-  <si>
-    <t>苏星河牛通</t>
-  </si>
-  <si>
-    <t>hanser</t>
-  </si>
-  <si>
-    <t>机智的Kason</t>
-  </si>
-  <si>
-    <t>中国BOY超级大猩猩</t>
-  </si>
-  <si>
-    <t>逍遥散人</t>
-  </si>
-  <si>
-    <t>和猫住</t>
-  </si>
-  <si>
-    <t>汪品先院士</t>
-  </si>
-  <si>
-    <t>电影最TOP</t>
-  </si>
-  <si>
-    <t>水无月菌</t>
-  </si>
-  <si>
-    <t>星有野</t>
-  </si>
-  <si>
-    <t>先看评测</t>
-  </si>
-  <si>
-    <t>DarkCarrot</t>
-  </si>
-  <si>
-    <t>浑元Rysn</t>
-  </si>
-  <si>
-    <t>老师好我叫何同学</t>
-  </si>
-  <si>
-    <t>帅soserious</t>
-  </si>
-  <si>
-    <t>柳青瑶本尊</t>
-  </si>
-  <si>
-    <t>某幻君</t>
-  </si>
-  <si>
-    <t>zettaranc</t>
-  </si>
-  <si>
-    <t>大漠叔叔</t>
-  </si>
-  <si>
-    <t>硬核的半佛仙人</t>
-  </si>
-  <si>
-    <t>画渣花小烙</t>
-  </si>
-  <si>
-    <t>MayTree五月树</t>
-  </si>
-  <si>
-    <t>翠花不太脆</t>
-  </si>
-  <si>
-    <t>记录生活的蛋黄派</t>
-  </si>
-  <si>
-    <t>刘谦</t>
-  </si>
-  <si>
-    <t>鹦鹉梨</t>
-  </si>
-  <si>
-    <t>狂阿弥_</t>
-  </si>
-  <si>
-    <t>青莲又失利了</t>
-  </si>
-  <si>
-    <t>凤凰传奇</t>
-  </si>
-  <si>
-    <t>罗翔说刑法</t>
-  </si>
-  <si>
-    <t>熊乐乐大魔王</t>
-  </si>
-  <si>
-    <t>帕梅拉PamelaReif</t>
-  </si>
-  <si>
-    <t>大象放映室</t>
-  </si>
-  <si>
-    <t>多多poi丶</t>
-  </si>
-  <si>
-    <t>森纳映画</t>
-  </si>
-  <si>
-    <t>泠鸢yousa</t>
-  </si>
-  <si>
-    <t>自来卷三木</t>
-  </si>
-  <si>
-    <t>田野上的繁荣</t>
-  </si>
-  <si>
-    <t>在下铁头阿彪</t>
-  </si>
-  <si>
-    <t>花少北丶</t>
-  </si>
-  <si>
-    <t>1900影剧室</t>
-  </si>
-  <si>
-    <t>塑料叉FOKU</t>
-  </si>
-  <si>
-    <t>火柴人AlanBecker</t>
-  </si>
-  <si>
-    <t>沙盘上的战争</t>
-  </si>
-  <si>
-    <t>杨可爱Ukulele</t>
-  </si>
-  <si>
-    <t>泛式</t>
-  </si>
-  <si>
-    <t>小片片说大片</t>
-  </si>
-  <si>
-    <t>香香软软的小泡芙</t>
-  </si>
-  <si>
-    <t>极客湾Geekerwan</t>
-  </si>
-  <si>
-    <t>=咬人猫=</t>
-  </si>
-  <si>
-    <t>日食记</t>
-  </si>
-  <si>
-    <t>啊吗粽</t>
-  </si>
-  <si>
-    <t>无穷小亮的科普日常</t>
-  </si>
-  <si>
-    <t>稚晖君</t>
-  </si>
-  <si>
-    <t>拜托了小翔哥</t>
-  </si>
-  <si>
-    <t>oooooohmygosh</t>
-  </si>
-  <si>
-    <t>兔叭咯</t>
-  </si>
-  <si>
-    <t>o小庄o</t>
-  </si>
-  <si>
-    <t>倒悬的橘子</t>
-  </si>
-  <si>
-    <t>取景框看世界</t>
-  </si>
-  <si>
-    <t>急速拍档</t>
-  </si>
-  <si>
-    <t>小文哥吃吃吃</t>
-  </si>
-  <si>
-    <t>木鱼水心</t>
-  </si>
-  <si>
-    <t>老番茄</t>
-  </si>
-  <si>
-    <t>大祥哥来了</t>
-  </si>
-  <si>
-    <t>魔法Zc目录</t>
-  </si>
-  <si>
-    <t>Vicky宣宣</t>
-  </si>
-  <si>
-    <t>远古黑金</t>
-  </si>
-  <si>
-    <t>好运的鱼</t>
-  </si>
-  <si>
-    <t>黑猫厨房</t>
-  </si>
-  <si>
-    <t>阿特警官</t>
-  </si>
-  <si>
-    <t>宝剑嫂</t>
-  </si>
-  <si>
-    <t>才疏学浅的才浅</t>
-  </si>
-  <si>
-    <t>朵朵花林</t>
-  </si>
-  <si>
-    <t>大碗拿铁</t>
-  </si>
-  <si>
-    <t>盗月社食遇记</t>
-  </si>
-  <si>
-    <t>导演小策</t>
-  </si>
-  <si>
-    <t>EdmundDZhang</t>
-  </si>
-  <si>
-    <t>二二酸酸</t>
-  </si>
-  <si>
-    <t>附魔星Fms</t>
-  </si>
-  <si>
-    <t>幾加乘</t>
-  </si>
-  <si>
-    <t>嘉然今天吃什么</t>
-  </si>
-  <si>
-    <t>九三的耳朵不是特别好</t>
-  </si>
-  <si>
-    <t>老爸评测</t>
-  </si>
-  <si>
-    <t>利维坦mY</t>
-  </si>
-  <si>
-    <t>绵羊料理</t>
-  </si>
-  <si>
-    <t>M木糖M</t>
-  </si>
-  <si>
-    <t>哦呼w</t>
-  </si>
-  <si>
-    <t>枪弹轨迹</t>
-  </si>
-  <si>
-    <t>RAY的模型世界</t>
-  </si>
-  <si>
-    <t>叔贵</t>
-  </si>
-  <si>
-    <t>我是郭杰瑞</t>
-  </si>
-  <si>
-    <t>小潮院长</t>
-  </si>
-  <si>
-    <t>小透明明TM</t>
-  </si>
-  <si>
-    <t>小约翰可汗</t>
-  </si>
-  <si>
-    <t>一鹿有车</t>
-  </si>
-  <si>
-    <t>影视飓风</t>
-  </si>
-  <si>
-    <t>共青团中央</t>
-  </si>
-  <si>
-    <t>在下哲别</t>
-  </si>
-  <si>
-    <t>雨哥到处跑</t>
-  </si>
-  <si>
-    <t>力元君</t>
-  </si>
-  <si>
-    <t>徐大虾咯</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -384,7 +63,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -392,7 +71,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="等线 Light"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -401,7 +80,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -410,7 +89,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -419,7 +98,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -427,7 +106,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -435,7 +114,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -443,7 +122,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -451,7 +130,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -460,7 +139,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -469,7 +148,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -477,7 +156,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -486,7 +165,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -494,7 +173,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -503,7 +182,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -512,7 +191,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -520,14 +199,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -964,48 +643,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1021,7 +700,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1316,22 +995,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G105"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1344,2607 +1022,2291 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>25503580</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
+      <c r="B2">
+        <v>587875.12</v>
       </c>
       <c r="C2">
-        <v>587875.12</v>
+        <v>29151.56</v>
       </c>
       <c r="D2">
-        <v>29151.56</v>
+        <v>8583.48</v>
       </c>
       <c r="E2">
-        <v>8583.48</v>
+        <f>D2/B2</f>
+        <v>1.460085604575339E-2</v>
       </c>
       <c r="F2">
-        <f>E2/C2</f>
-        <v>1.460085604575339E-2</v>
-      </c>
-      <c r="G2">
-        <f>D2/C2</f>
+        <f>C2/B2</f>
         <v>4.9588014542952592E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>598464467</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
+      <c r="B3">
+        <v>1583288.19318181</v>
       </c>
       <c r="C3">
-        <v>1583288.19318181</v>
+        <v>91661.420454545398</v>
       </c>
       <c r="D3">
-        <v>91661.420454545398</v>
+        <v>42437.784090909001</v>
       </c>
       <c r="E3">
-        <v>42437.784090909001</v>
+        <f t="shared" ref="E3:E66" si="0">D3/B3</f>
+        <v>2.6803575163170463E-2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F66" si="0">E3/C3</f>
-        <v>2.6803575163170463E-2</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G66" si="1">D3/C3</f>
+        <f t="shared" ref="F3:F66" si="1">C3/B3</f>
         <v>5.7893073951584668E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>11073</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
+      <c r="B4">
+        <v>1443508.44927536</v>
       </c>
       <c r="C4">
-        <v>1443508.44927536</v>
+        <v>96258.442028985504</v>
       </c>
       <c r="D4">
-        <v>96258.442028985504</v>
+        <v>44751.036231883998</v>
       </c>
       <c r="E4">
-        <v>44751.036231883998</v>
+        <f t="shared" si="0"/>
+        <v>3.1001575539338879E-2</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
-        <v>3.1001575539338879E-2</v>
-      </c>
-      <c r="G4">
         <f t="shared" si="1"/>
         <v>6.6683670661787375E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>8549577</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
+      <c r="B5">
+        <v>2153011.5094339601</v>
       </c>
       <c r="C5">
-        <v>2153011.5094339601</v>
+        <v>141712.03144654</v>
       </c>
       <c r="D5">
-        <v>141712.03144654</v>
+        <v>62703.056603773497</v>
       </c>
       <c r="E5">
-        <v>62703.056603773497</v>
+        <f t="shared" si="0"/>
+        <v>2.9123419140596473E-2</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
-        <v>2.9123419140596473E-2</v>
-      </c>
-      <c r="G5">
         <f t="shared" si="1"/>
         <v>6.5820378026588883E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>562197</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
+      <c r="B6">
+        <v>2006732.0191387499</v>
       </c>
       <c r="C6">
-        <v>2006732.0191387499</v>
+        <v>140376.277511961</v>
       </c>
       <c r="D6">
-        <v>140376.277511961</v>
+        <v>59116.354066985601</v>
       </c>
       <c r="E6">
-        <v>59116.354066985601</v>
+        <f t="shared" si="0"/>
+        <v>2.9459017698016888E-2</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
-        <v>2.9459017698016888E-2</v>
-      </c>
-      <c r="G6">
         <f t="shared" si="1"/>
         <v>6.9952677374534422E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>168598</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
+      <c r="B7">
+        <v>1861985.2741312699</v>
       </c>
       <c r="C7">
-        <v>1861985.2741312699</v>
+        <v>130058.594594594</v>
       </c>
       <c r="D7">
-        <v>130058.594594594</v>
+        <v>56505.876447876399</v>
       </c>
       <c r="E7">
-        <v>56505.876447876399</v>
+        <f t="shared" si="0"/>
+        <v>3.0347112425064611E-2</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
-        <v>3.0347112425064611E-2</v>
-      </c>
-      <c r="G7">
         <f t="shared" si="1"/>
         <v>6.9849421690659885E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>26321770</v>
       </c>
-      <c r="B8" t="s">
-        <v>11</v>
+      <c r="B8">
+        <v>1735972.2621359201</v>
       </c>
       <c r="C8">
-        <v>1735972.2621359201</v>
+        <v>127822.31067961099</v>
       </c>
       <c r="D8">
-        <v>127822.31067961099</v>
+        <v>54072.184466019396</v>
       </c>
       <c r="E8">
-        <v>54072.184466019396</v>
+        <f t="shared" si="0"/>
+        <v>3.1148069381874574E-2</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
-        <v>3.1148069381874574E-2</v>
-      </c>
-      <c r="G8">
         <f t="shared" si="1"/>
         <v>7.3631539781828029E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>513722566</v>
       </c>
-      <c r="B9" t="s">
-        <v>12</v>
+      <c r="B9">
+        <v>1549738.49582172</v>
       </c>
       <c r="C9">
-        <v>1549738.49582172</v>
+        <v>115993.456824512</v>
       </c>
       <c r="D9">
-        <v>115993.456824512</v>
+        <v>48527.849582172697</v>
       </c>
       <c r="E9">
-        <v>48527.849582172697</v>
+        <f t="shared" si="0"/>
+        <v>3.1313573040231996E-2</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
-        <v>3.1313573040231996E-2</v>
-      </c>
-      <c r="G9">
         <f t="shared" si="1"/>
         <v>7.4847115908422107E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>17819768</v>
       </c>
-      <c r="B10" t="s">
-        <v>13</v>
+      <c r="B10">
+        <v>1514924.19559902</v>
       </c>
       <c r="C10">
-        <v>1514924.19559902</v>
+        <v>109768.22982885</v>
       </c>
       <c r="D10">
-        <v>109768.22982885</v>
+        <v>46774.154034229803</v>
       </c>
       <c r="E10">
-        <v>46774.154034229803</v>
+        <f t="shared" si="0"/>
+        <v>3.087557395288331E-2</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
-        <v>3.087557395288331E-2</v>
-      </c>
-      <c r="G10">
         <f t="shared" si="1"/>
         <v>7.2457902611718653E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1958342</v>
       </c>
-      <c r="B11" t="s">
-        <v>14</v>
+      <c r="B11">
+        <v>1932397.4901960699</v>
       </c>
       <c r="C11">
-        <v>1932397.4901960699</v>
+        <v>121698.901960784</v>
       </c>
       <c r="D11">
-        <v>121698.901960784</v>
+        <v>57797.228758169898</v>
       </c>
       <c r="E11">
-        <v>57797.228758169898</v>
+        <f t="shared" si="0"/>
+        <v>2.9909596266503909E-2</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
-        <v>2.9909596266503909E-2</v>
-      </c>
-      <c r="G11">
         <f t="shared" si="1"/>
         <v>6.2978192932984955E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>627888730</v>
       </c>
-      <c r="B12" t="s">
-        <v>15</v>
+      <c r="B12">
+        <v>2244759.25343811</v>
       </c>
       <c r="C12">
-        <v>2244759.25343811</v>
+        <v>148424.27897838899</v>
       </c>
       <c r="D12">
-        <v>148424.27897838899</v>
+        <v>61200.962671905698</v>
       </c>
       <c r="E12">
-        <v>61200.962671905698</v>
+        <f t="shared" si="0"/>
+        <v>2.7263931567792537E-2</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
-        <v>2.7263931567792537E-2</v>
-      </c>
-      <c r="G12">
         <f t="shared" si="1"/>
         <v>6.6120355112050402E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>483311105</v>
       </c>
-      <c r="B13" t="s">
-        <v>16</v>
+      <c r="B13">
+        <v>2099948.3381037498</v>
       </c>
       <c r="C13">
-        <v>2099948.3381037498</v>
+        <v>138502.05187835399</v>
       </c>
       <c r="D13">
-        <v>138502.05187835399</v>
+        <v>58292.581395348803</v>
       </c>
       <c r="E13">
-        <v>58292.581395348803</v>
+        <f t="shared" si="0"/>
+        <v>2.7759054990841782E-2</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
-        <v>2.7759054990841782E-2</v>
-      </c>
-      <c r="G13">
         <f t="shared" si="1"/>
         <v>6.59549805893897E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>21869937</v>
       </c>
-      <c r="B14" t="s">
-        <v>17</v>
+      <c r="B14">
+        <v>2020060.77504105</v>
       </c>
       <c r="C14">
-        <v>2020060.77504105</v>
+        <v>131757.79638752001</v>
       </c>
       <c r="D14">
-        <v>131757.79638752001</v>
+        <v>55911.711001641997</v>
       </c>
       <c r="E14">
-        <v>55911.711001641997</v>
+        <f t="shared" si="0"/>
+        <v>2.7678232106905697E-2</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
-        <v>2.7678232106905697E-2</v>
-      </c>
-      <c r="G14">
         <f t="shared" si="1"/>
         <v>6.5224669482947875E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>42561463</v>
       </c>
-      <c r="B15" t="s">
-        <v>18</v>
+      <c r="B15">
+        <v>1957500.9772382299</v>
       </c>
       <c r="C15">
-        <v>1957500.9772382299</v>
+        <v>132318.44916540201</v>
       </c>
       <c r="D15">
-        <v>132318.44916540201</v>
+        <v>53129.511380880103</v>
       </c>
       <c r="E15">
-        <v>53129.511380880103</v>
+        <f t="shared" si="0"/>
+        <v>2.7141499288464561E-2</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
-        <v>2.7141499288464561E-2</v>
-      </c>
-      <c r="G15">
         <f t="shared" si="1"/>
         <v>6.759559801195375E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>163637592</v>
       </c>
-      <c r="B16" t="s">
-        <v>19</v>
+      <c r="B16">
+        <v>2304991.3588652401</v>
       </c>
       <c r="C16">
-        <v>2304991.3588652401</v>
+        <v>171528.723404255</v>
       </c>
       <c r="D16">
-        <v>171528.723404255</v>
+        <v>92784.357446808499</v>
       </c>
       <c r="E16">
-        <v>92784.357446808499</v>
+        <f t="shared" si="0"/>
+        <v>4.0253668236086899E-2</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
-        <v>4.0253668236086899E-2</v>
-      </c>
-      <c r="G16">
         <f t="shared" si="1"/>
         <v>7.4416211038942692E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>66391032</v>
       </c>
-      <c r="B17" t="s">
-        <v>20</v>
+      <c r="B17">
+        <v>2303657.2476821099</v>
       </c>
       <c r="C17">
-        <v>2303657.2476821099</v>
+        <v>167206.038410596</v>
       </c>
       <c r="D17">
-        <v>167206.038410596</v>
+        <v>90834.241059602602</v>
       </c>
       <c r="E17">
-        <v>90834.241059602602</v>
+        <f t="shared" si="0"/>
+        <v>3.9430449625697597E-2</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
-        <v>3.9430449625697597E-2</v>
-      </c>
-      <c r="G17">
         <f t="shared" si="1"/>
         <v>7.2582863001357995E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>30954515</v>
       </c>
-      <c r="B18" t="s">
-        <v>21</v>
+      <c r="B18">
+        <v>2185034.6993788802</v>
       </c>
       <c r="C18">
-        <v>2185034.6993788802</v>
+        <v>159539.11180124199</v>
       </c>
       <c r="D18">
-        <v>159539.11180124199</v>
+        <v>86142.521739130403</v>
       </c>
       <c r="E18">
-        <v>86142.521739130403</v>
+        <f t="shared" si="0"/>
+        <v>3.9423868995589563E-2</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
-        <v>3.9423868995589563E-2</v>
-      </c>
-      <c r="G18">
         <f t="shared" si="1"/>
         <v>7.3014452286086218E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1577804</v>
       </c>
-      <c r="B19" t="s">
-        <v>22</v>
+      <c r="B19">
+        <v>2215571.4549707598</v>
       </c>
       <c r="C19">
-        <v>2215571.4549707598</v>
+        <v>165874.61637426901</v>
       </c>
       <c r="D19">
-        <v>165874.61637426901</v>
+        <v>89161.922807017501</v>
       </c>
       <c r="E19">
-        <v>89161.922807017501</v>
+        <f t="shared" si="0"/>
+        <v>4.0243307254648766E-2</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
-        <v>4.0243307254648766E-2</v>
-      </c>
-      <c r="G19">
         <f t="shared" si="1"/>
         <v>7.4867644644057832E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>326246517</v>
       </c>
-      <c r="B20" t="s">
-        <v>23</v>
+      <c r="B20">
+        <v>2123729.4165745801</v>
       </c>
       <c r="C20">
-        <v>2123729.4165745801</v>
+        <v>158033.48950276201</v>
       </c>
       <c r="D20">
-        <v>158033.48950276201</v>
+        <v>84642.173480662896</v>
       </c>
       <c r="E20">
-        <v>84642.173480662896</v>
+        <f t="shared" si="0"/>
+        <v>3.9855441479538629E-2</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
-        <v>3.9855441479538629E-2</v>
-      </c>
-      <c r="G20">
         <f t="shared" si="1"/>
         <v>7.4413194199503263E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>67141499</v>
       </c>
-      <c r="B21" t="s">
-        <v>24</v>
+      <c r="B21">
+        <v>2135660.4670156999</v>
       </c>
       <c r="C21">
-        <v>2135660.4670156999</v>
+        <v>161244.040837696</v>
       </c>
       <c r="D21">
-        <v>161244.040837696</v>
+        <v>83847.047120418807</v>
       </c>
       <c r="E21">
-        <v>83847.047120418807</v>
+        <f t="shared" si="0"/>
+        <v>3.9260476286094227E-2</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
-        <v>3.9260476286094227E-2</v>
-      </c>
-      <c r="G21">
         <f t="shared" si="1"/>
         <v>7.5500784571347609E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>37663924</v>
       </c>
-      <c r="B22" t="s">
-        <v>25</v>
+      <c r="B22">
+        <v>2118468.3960199002</v>
       </c>
       <c r="C22">
-        <v>2118468.3960199002</v>
+        <v>157886.28258706399</v>
       </c>
       <c r="D22">
-        <v>157886.28258706399</v>
+        <v>80558.726368159201</v>
       </c>
       <c r="E22">
-        <v>80558.726368159201</v>
+        <f t="shared" si="0"/>
+        <v>3.8026871922899559E-2</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
-        <v>3.8026871922899559E-2</v>
-      </c>
-      <c r="G22">
         <f t="shared" si="1"/>
         <v>7.4528505067007311E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>402576555</v>
       </c>
-      <c r="B23" t="s">
-        <v>26</v>
+      <c r="B23">
+        <v>2157002.12132701</v>
       </c>
       <c r="C23">
-        <v>2157002.12132701</v>
+        <v>160222.88909952599</v>
       </c>
       <c r="D23">
-        <v>160222.88909952599</v>
+        <v>77938.2464454976</v>
       </c>
       <c r="E23">
-        <v>77938.2464454976</v>
+        <f t="shared" si="0"/>
+        <v>3.6132670281079367E-2</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
-        <v>3.6132670281079367E-2</v>
-      </c>
-      <c r="G23">
         <f t="shared" si="1"/>
         <v>7.428035768502407E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1468951948</v>
       </c>
-      <c r="B24" t="s">
-        <v>27</v>
+      <c r="B24">
+        <v>2102275.06968325</v>
       </c>
       <c r="C24">
-        <v>2102275.06968325</v>
+        <v>154846.33484162801</v>
       </c>
       <c r="D24">
-        <v>154846.33484162801</v>
+        <v>74631.821719457002</v>
       </c>
       <c r="E24">
-        <v>74631.821719457002</v>
+        <f t="shared" si="0"/>
+        <v>3.5500502667665551E-2</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
-        <v>3.5500502667665551E-2</v>
-      </c>
-      <c r="G24">
         <f t="shared" si="1"/>
         <v>7.3656552881521217E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>337312411</v>
       </c>
-      <c r="B25" t="s">
-        <v>28</v>
+      <c r="B25">
+        <v>2115550.4787878701</v>
       </c>
       <c r="C25">
-        <v>2115550.4787878701</v>
+        <v>157068.25454545399</v>
       </c>
       <c r="D25">
-        <v>157068.25454545399</v>
+        <v>76473.339393939401</v>
       </c>
       <c r="E25">
-        <v>76473.339393939401</v>
+        <f t="shared" si="0"/>
+        <v>3.6148198854491866E-2</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
-        <v>3.6148198854491866E-2</v>
-      </c>
-      <c r="G25">
         <f t="shared" si="1"/>
         <v>7.4244626219199514E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>337521240</v>
       </c>
-      <c r="B26" t="s">
-        <v>29</v>
+      <c r="B26">
+        <v>2155421.3958506202</v>
       </c>
       <c r="C26">
-        <v>2155421.3958506202</v>
+        <v>162250.990041493</v>
       </c>
       <c r="D26">
-        <v>162250.990041493</v>
+        <v>76129.518672199105</v>
       </c>
       <c r="E26">
-        <v>76129.518672199105</v>
+        <f t="shared" si="0"/>
+        <v>3.5320016224556029E-2</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
-        <v>3.5320016224556029E-2</v>
-      </c>
-      <c r="G26">
         <f t="shared" si="1"/>
         <v>7.5275762945399324E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>641975239</v>
       </c>
-      <c r="B27" t="s">
-        <v>30</v>
+      <c r="B27">
+        <v>2143222.0087649398</v>
       </c>
       <c r="C27">
-        <v>2143222.0087649398</v>
+        <v>161120.5625498</v>
       </c>
       <c r="D27">
-        <v>161120.5625498</v>
+        <v>75098.651792828605</v>
       </c>
       <c r="E27">
-        <v>75098.651792828605</v>
+        <f t="shared" si="0"/>
+        <v>3.504007120387178E-2</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
-        <v>3.504007120387178E-2</v>
-      </c>
-      <c r="G27">
         <f t="shared" si="1"/>
         <v>7.5176795446705899E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1968595</v>
       </c>
-      <c r="B28" t="s">
-        <v>31</v>
+      <c r="B28">
+        <v>2090715.9026819901</v>
       </c>
       <c r="C28">
-        <v>2090715.9026819901</v>
+        <v>156942.41915708801</v>
       </c>
       <c r="D28">
-        <v>156942.41915708801</v>
+        <v>72852.560153256694</v>
       </c>
       <c r="E28">
-        <v>72852.560153256694</v>
+        <f t="shared" si="0"/>
+        <v>3.4845748319894038E-2</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
-        <v>3.4845748319894038E-2</v>
-      </c>
-      <c r="G28">
         <f t="shared" si="1"/>
         <v>7.5066353566144869E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3433092</v>
       </c>
-      <c r="B29" t="s">
-        <v>32</v>
+      <c r="B29">
+        <v>2056103.55571955</v>
       </c>
       <c r="C29">
-        <v>2056103.55571955</v>
+        <v>154932.13431734301</v>
       </c>
       <c r="D29">
-        <v>154932.13431734301</v>
+        <v>73084.407380073797</v>
       </c>
       <c r="E29">
-        <v>73084.407380073797</v>
+        <f t="shared" si="0"/>
+        <v>3.5545100428804675E-2</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
-        <v>3.5545100428804675E-2</v>
-      </c>
-      <c r="G29">
         <f t="shared" si="1"/>
         <v>7.5352301145709205E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>179922650</v>
       </c>
-      <c r="B30" t="s">
-        <v>33</v>
+      <c r="B30">
+        <v>2084955.0975088901</v>
       </c>
       <c r="C30">
-        <v>2084955.0975088901</v>
+        <v>156238.17651245499</v>
       </c>
       <c r="D30">
-        <v>156238.17651245499</v>
+        <v>71979.651957295297</v>
       </c>
       <c r="E30">
-        <v>71979.651957295297</v>
+        <f t="shared" si="0"/>
+        <v>3.4523358341528206E-2</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
-        <v>3.4523358341528206E-2</v>
-      </c>
-      <c r="G30">
         <f t="shared" si="1"/>
         <v>7.4935991043226194E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1646036311</v>
       </c>
-      <c r="B31" t="s">
-        <v>34</v>
+      <c r="B31">
+        <v>2076203.8701030901</v>
       </c>
       <c r="C31">
-        <v>2076203.8701030901</v>
+        <v>155691.070790378</v>
       </c>
       <c r="D31">
-        <v>155691.070790378</v>
+        <v>72422.039175257698</v>
       </c>
       <c r="E31">
-        <v>72422.039175257698</v>
+        <f t="shared" si="0"/>
+        <v>3.4881949801809066E-2</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
-        <v>3.4881949801809066E-2</v>
-      </c>
-      <c r="G31">
         <f t="shared" si="1"/>
         <v>7.4988334735474435E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>517327498</v>
       </c>
-      <c r="B32" t="s">
-        <v>35</v>
+      <c r="B32">
+        <v>2081614.93687707</v>
       </c>
       <c r="C32">
-        <v>2081614.93687707</v>
+        <v>157452.53156146099</v>
       </c>
       <c r="D32">
-        <v>157452.53156146099</v>
+        <v>72386.342857142794</v>
       </c>
       <c r="E32">
-        <v>72386.342857142794</v>
+        <f t="shared" si="0"/>
+        <v>3.4774127325267926E-2</v>
       </c>
       <c r="F32">
-        <f t="shared" si="0"/>
-        <v>3.4774127325267926E-2</v>
-      </c>
-      <c r="G32">
         <f t="shared" si="1"/>
         <v>7.5639604987499845E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>107278647</v>
       </c>
-      <c r="B33" t="s">
-        <v>36</v>
+      <c r="B33">
+        <v>2076870.1627009599</v>
       </c>
       <c r="C33">
-        <v>2076870.1627009599</v>
+        <v>155288.66045016001</v>
       </c>
       <c r="D33">
-        <v>155288.66045016001</v>
+        <v>70652.756270096404</v>
       </c>
       <c r="E33">
-        <v>70652.756270096404</v>
+        <f t="shared" si="0"/>
+        <v>3.4018860465602159E-2</v>
       </c>
       <c r="F33">
-        <f t="shared" si="0"/>
-        <v>3.4018860465602159E-2</v>
-      </c>
-      <c r="G33">
         <f t="shared" si="1"/>
         <v>7.4770519235640528E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>604003146</v>
       </c>
-      <c r="B34" t="s">
-        <v>37</v>
+      <c r="B34">
+        <v>2052224.1152647899</v>
       </c>
       <c r="C34">
-        <v>2052224.1152647899</v>
+        <v>151050.76884735201</v>
       </c>
       <c r="D34">
-        <v>151050.76884735201</v>
+        <v>68622.153894080999</v>
       </c>
       <c r="E34">
-        <v>68622.153894080999</v>
+        <f t="shared" si="0"/>
+        <v>3.3437943440805425E-2</v>
       </c>
       <c r="F34">
-        <f t="shared" si="0"/>
-        <v>3.3437943440805425E-2</v>
-      </c>
-      <c r="G34">
         <f t="shared" si="1"/>
         <v>7.360344697433914E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>49246269</v>
       </c>
-      <c r="B35" t="s">
-        <v>38</v>
+      <c r="B35">
+        <v>2014988.755287</v>
       </c>
       <c r="C35">
-        <v>2014988.755287</v>
+        <v>147913.56918429001</v>
       </c>
       <c r="D35">
-        <v>147913.56918429001</v>
+        <v>67701.338368580007</v>
       </c>
       <c r="E35">
-        <v>67701.338368580007</v>
+        <f t="shared" si="0"/>
+        <v>3.3598866589673419E-2</v>
       </c>
       <c r="F35">
-        <f t="shared" si="0"/>
-        <v>3.3598866589673419E-2</v>
-      </c>
-      <c r="G35">
         <f t="shared" si="1"/>
         <v>7.3406647454577131E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>11253297</v>
       </c>
-      <c r="B36" t="s">
-        <v>39</v>
+      <c r="B36">
+        <v>1968464.3953079099</v>
       </c>
       <c r="C36">
-        <v>1968464.3953079099</v>
+        <v>144740.53372434</v>
       </c>
       <c r="D36">
-        <v>144740.53372434</v>
+        <v>66022.368914955994</v>
       </c>
       <c r="E36">
-        <v>66022.368914955994</v>
+        <f t="shared" si="0"/>
+        <v>3.3540037133680888E-2</v>
       </c>
       <c r="F36">
-        <f t="shared" si="0"/>
-        <v>3.3540037133680888E-2</v>
-      </c>
-      <c r="G36">
         <f t="shared" si="1"/>
         <v>7.3529668135907278E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1724598</v>
       </c>
-      <c r="B37" t="s">
-        <v>40</v>
+      <c r="B37">
+        <v>1943102.1105413099</v>
       </c>
       <c r="C37">
-        <v>1943102.1105413099</v>
+        <v>142640.50541310501</v>
       </c>
       <c r="D37">
-        <v>142640.50541310501</v>
+        <v>64738.7606837606</v>
       </c>
       <c r="E37">
-        <v>64738.7606837606</v>
+        <f t="shared" si="0"/>
+        <v>3.3317220094895406E-2</v>
       </c>
       <c r="F37">
-        <f t="shared" si="0"/>
-        <v>3.3317220094895406E-2</v>
-      </c>
-      <c r="G37">
         <f t="shared" si="1"/>
         <v>7.3408651372092931E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>282994</v>
       </c>
-      <c r="B38" t="s">
-        <v>41</v>
+      <c r="B38">
+        <v>1903661.9883656499</v>
       </c>
       <c r="C38">
-        <v>1903661.9883656499</v>
+        <v>140140.68864265899</v>
       </c>
       <c r="D38">
-        <v>140140.68864265899</v>
+        <v>63577.121883656502</v>
       </c>
       <c r="E38">
-        <v>63577.121883656502</v>
+        <f t="shared" si="0"/>
+        <v>3.339727444904194E-2</v>
       </c>
       <c r="F38">
-        <f t="shared" si="0"/>
-        <v>3.339727444904194E-2</v>
-      </c>
-      <c r="G38">
         <f t="shared" si="1"/>
         <v>7.3616371760920604E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>474702359</v>
       </c>
-      <c r="B39" t="s">
-        <v>42</v>
+      <c r="B39">
+        <v>1911082.78598382</v>
       </c>
       <c r="C39">
-        <v>1911082.78598382</v>
+        <v>141879.93908355699</v>
       </c>
       <c r="D39">
-        <v>141879.93908355699</v>
+        <v>63397.149326145503</v>
       </c>
       <c r="E39">
-        <v>63397.149326145503</v>
+        <f t="shared" si="0"/>
+        <v>3.3173418645759414E-2</v>
       </c>
       <c r="F39">
-        <f t="shared" si="0"/>
-        <v>3.3173418645759414E-2</v>
-      </c>
-      <c r="G39">
         <f t="shared" si="1"/>
         <v>7.4240603350167064E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>588278127</v>
       </c>
-      <c r="B40" t="s">
-        <v>43</v>
+      <c r="B40">
+        <v>1885176.8488188901</v>
       </c>
       <c r="C40">
-        <v>1885176.8488188901</v>
+        <v>139338.39842519601</v>
       </c>
       <c r="D40">
-        <v>139338.39842519601</v>
+        <v>61983.705511811</v>
       </c>
       <c r="E40">
-        <v>61983.705511811</v>
+        <f t="shared" si="0"/>
+        <v>3.2879517669997554E-2</v>
       </c>
       <c r="F40">
-        <f t="shared" si="0"/>
-        <v>3.2879517669997554E-2</v>
-      </c>
-      <c r="G40">
         <f t="shared" si="1"/>
         <v>7.3912640351219541E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>27565758</v>
       </c>
-      <c r="B41" t="e" cm="1">
-        <f t="array" ref="B41">-小D-biu</f>
-        <v>#NAME?</v>
+      <c r="B41">
+        <v>1854536.1207161101</v>
       </c>
       <c r="C41">
-        <v>1854536.1207161101</v>
+        <v>137131.701278772</v>
       </c>
       <c r="D41">
-        <v>137131.701278772</v>
+        <v>60689.251150895099</v>
       </c>
       <c r="E41">
-        <v>60689.251150895099</v>
+        <f t="shared" si="0"/>
+        <v>3.2724760910809635E-2</v>
       </c>
       <c r="F41">
-        <f t="shared" si="0"/>
-        <v>3.2724760910809635E-2</v>
-      </c>
-      <c r="G41">
         <f t="shared" si="1"/>
         <v>7.3943936570952315E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>335575297</v>
       </c>
-      <c r="B42" t="s">
-        <v>44</v>
+      <c r="B42">
+        <v>1896611.7193596701</v>
       </c>
       <c r="C42">
-        <v>1896611.7193596701</v>
+        <v>136904.44422211099</v>
       </c>
       <c r="D42">
-        <v>136904.44422211099</v>
+        <v>59871.759879939898</v>
       </c>
       <c r="E42">
-        <v>59871.759879939898</v>
+        <f t="shared" si="0"/>
+        <v>3.1567747509307638E-2</v>
       </c>
       <c r="F42">
-        <f t="shared" si="0"/>
-        <v>3.1567747509307638E-2</v>
-      </c>
-      <c r="G42">
         <f t="shared" si="1"/>
         <v>7.2183696232949762E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2206456</v>
       </c>
-      <c r="B43" t="s">
-        <v>45</v>
+      <c r="B43">
+        <v>1920112.80868716</v>
       </c>
       <c r="C43">
-        <v>1920112.80868716</v>
+        <v>139706.654465592</v>
       </c>
       <c r="D43">
-        <v>139706.654465592</v>
+        <v>61277.095168374799</v>
       </c>
       <c r="E43">
-        <v>61277.095168374799</v>
+        <f t="shared" si="0"/>
+        <v>3.1913278684012232E-2</v>
       </c>
       <c r="F43">
-        <f t="shared" si="0"/>
-        <v>3.1913278684012232E-2</v>
-      </c>
-      <c r="G43">
         <f t="shared" si="1"/>
         <v>7.2759607578011906E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>17223352</v>
       </c>
-      <c r="B44" t="s">
-        <v>46</v>
+      <c r="B44">
+        <v>1882948.3449261501</v>
       </c>
       <c r="C44">
-        <v>1882948.3449261501</v>
+        <v>136899.580276322</v>
       </c>
       <c r="D44">
-        <v>136899.580276322</v>
+        <v>60043.787994282902</v>
       </c>
       <c r="E44">
-        <v>60043.787994282902</v>
+        <f t="shared" si="0"/>
+        <v>3.1888175879109332E-2</v>
       </c>
       <c r="F44">
-        <f t="shared" si="0"/>
-        <v>3.1888175879109332E-2</v>
-      </c>
-      <c r="G44">
         <f t="shared" si="1"/>
         <v>7.2704904861153399E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>130636947</v>
       </c>
-      <c r="B45" t="s">
-        <v>47</v>
+      <c r="B45">
+        <v>1867360.5523499299</v>
       </c>
       <c r="C45">
-        <v>1867360.5523499299</v>
+        <v>135643.611447184</v>
       </c>
       <c r="D45">
-        <v>135643.611447184</v>
+        <v>59124.933922754703</v>
       </c>
       <c r="E45">
-        <v>59124.933922754703</v>
+        <f t="shared" si="0"/>
+        <v>3.1662302091768249E-2</v>
       </c>
       <c r="F45">
-        <f t="shared" si="0"/>
-        <v>3.1662302091768249E-2</v>
-      </c>
-      <c r="G45">
         <f t="shared" si="1"/>
         <v>7.2639218642852305E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>519253600</v>
       </c>
-      <c r="B46" t="s">
-        <v>48</v>
+      <c r="B46">
+        <v>1837925.6161891699</v>
       </c>
       <c r="C46">
-        <v>1837925.6161891699</v>
+        <v>133475.238744884</v>
       </c>
       <c r="D46">
-        <v>133475.238744884</v>
+        <v>57992.290131878101</v>
       </c>
       <c r="E46">
-        <v>57992.290131878101</v>
+        <f t="shared" si="0"/>
+        <v>3.1553121421813407E-2</v>
       </c>
       <c r="F46">
-        <f t="shared" si="0"/>
-        <v>3.1553121421813407E-2</v>
-      </c>
-      <c r="G46">
         <f t="shared" si="1"/>
         <v>7.2622764256171049E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>612194373</v>
       </c>
-      <c r="B47" t="s">
-        <v>49</v>
+      <c r="B47">
+        <v>1813931.91196087</v>
       </c>
       <c r="C47">
-        <v>1813931.91196087</v>
+        <v>131537.51311694001</v>
       </c>
       <c r="D47">
-        <v>131537.51311694001</v>
+        <v>57244.715873721601</v>
       </c>
       <c r="E47">
-        <v>57244.715873721601</v>
+        <f t="shared" si="0"/>
+        <v>3.1558359768774212E-2</v>
       </c>
       <c r="F47">
-        <f t="shared" si="0"/>
-        <v>3.1558359768774212E-2</v>
-      </c>
-      <c r="G47">
         <f t="shared" si="1"/>
         <v>7.2515132596541215E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>249608727</v>
       </c>
-      <c r="B48" t="s">
-        <v>50</v>
+      <c r="B48">
+        <v>1800478.73118747</v>
       </c>
       <c r="C48">
-        <v>1800478.73118747</v>
+        <v>130399.253588516</v>
       </c>
       <c r="D48">
-        <v>130399.253588516</v>
+        <v>57409.029143105698</v>
       </c>
       <c r="E48">
-        <v>57409.029143105698</v>
+        <f t="shared" si="0"/>
+        <v>3.1885424775466638E-2</v>
       </c>
       <c r="F48">
-        <f t="shared" si="0"/>
-        <v>3.1885424775466638E-2</v>
-      </c>
-      <c r="G48">
         <f t="shared" si="1"/>
         <v>7.2424767551968666E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>63231</v>
       </c>
-      <c r="B49" t="s">
-        <v>51</v>
+      <c r="B49">
+        <v>1826483.82205193</v>
       </c>
       <c r="C49">
-        <v>1826483.82205193</v>
+        <v>132434.369944657</v>
       </c>
       <c r="D49">
-        <v>132434.369944657</v>
+        <v>58084.554278416297</v>
       </c>
       <c r="E49">
-        <v>58084.554278416297</v>
+        <f t="shared" si="0"/>
+        <v>3.1801296883737118E-2</v>
       </c>
       <c r="F49">
-        <f t="shared" si="0"/>
-        <v>3.1801296883737118E-2</v>
-      </c>
-      <c r="G49">
         <f t="shared" si="1"/>
         <v>7.2507825333966561E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>10119428</v>
       </c>
-      <c r="B50" t="s">
-        <v>52</v>
+      <c r="B50">
+        <v>1815856.76365152</v>
       </c>
       <c r="C50">
-        <v>1815856.76365152</v>
+        <v>131336.44935389701</v>
       </c>
       <c r="D50">
-        <v>131336.44935389701</v>
+        <v>57384.5452271779</v>
       </c>
       <c r="E50">
-        <v>57384.5452271779</v>
+        <f t="shared" si="0"/>
+        <v>3.1601911767414344E-2</v>
       </c>
       <c r="F50">
-        <f t="shared" si="0"/>
-        <v>3.1601911767414344E-2</v>
-      </c>
-      <c r="G50">
         <f t="shared" si="1"/>
         <v>7.232753815328008E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>298946431</v>
       </c>
-      <c r="B51" t="s">
-        <v>53</v>
+      <c r="B51">
+        <v>1786228.20498162</v>
       </c>
       <c r="C51">
-        <v>1786228.20498162</v>
+        <v>129344.830543078</v>
       </c>
       <c r="D51">
-        <v>129344.830543078</v>
+        <v>56261.961616986497</v>
       </c>
       <c r="E51">
-        <v>56261.961616986497</v>
+        <f t="shared" si="0"/>
+        <v>3.1497633650659676E-2</v>
       </c>
       <c r="F51">
-        <f t="shared" si="0"/>
-        <v>3.1497633650659676E-2</v>
-      </c>
-      <c r="G51">
         <f t="shared" si="1"/>
         <v>7.2412265231479173E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>25876945</v>
       </c>
-      <c r="B52" t="s">
-        <v>54</v>
+      <c r="B52">
+        <v>1771101.0764305701</v>
       </c>
       <c r="C52">
-        <v>1771101.0764305701</v>
+        <v>127970.28531412499</v>
       </c>
       <c r="D52">
-        <v>127970.28531412499</v>
+        <v>55756.337334933902</v>
       </c>
       <c r="E52">
-        <v>55756.337334933902</v>
+        <f t="shared" si="0"/>
+        <v>3.1481171841024308E-2</v>
       </c>
       <c r="F52">
-        <f t="shared" si="0"/>
-        <v>3.1481171841024308E-2</v>
-      </c>
-      <c r="G52">
         <f t="shared" si="1"/>
         <v>7.2254648262104218E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>116683</v>
       </c>
-      <c r="B53" t="s">
-        <v>55</v>
+      <c r="B53">
+        <v>1803598.7406826201</v>
       </c>
       <c r="C53">
-        <v>1803598.7406826201</v>
+        <v>128353.480580619</v>
       </c>
       <c r="D53">
-        <v>128353.480580619</v>
+        <v>56050.767752059597</v>
       </c>
       <c r="E53">
-        <v>56050.767752059597</v>
+        <f t="shared" si="0"/>
+        <v>3.1077182794464409E-2</v>
       </c>
       <c r="F53">
-        <f t="shared" si="0"/>
-        <v>3.1077182794464409E-2</v>
-      </c>
-      <c r="G53">
         <f t="shared" si="1"/>
         <v>7.1165208582946893E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>8960728</v>
       </c>
-      <c r="B54" t="s">
-        <v>56</v>
+      <c r="B54">
+        <v>1800945.7926125401</v>
       </c>
       <c r="C54">
-        <v>1800945.7926125401</v>
+        <v>128297.881108118</v>
       </c>
       <c r="D54">
-        <v>128297.881108118</v>
+        <v>55851.395536744902</v>
       </c>
       <c r="E54">
-        <v>55851.395536744902</v>
+        <f t="shared" si="0"/>
+        <v>3.1012257984580498E-2</v>
       </c>
       <c r="F54">
-        <f t="shared" si="0"/>
-        <v>3.1012257984580498E-2</v>
-      </c>
-      <c r="G54">
         <f t="shared" si="1"/>
         <v>7.1239168682585841E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>7552204</v>
       </c>
-      <c r="B55" t="s">
-        <v>57</v>
+      <c r="B55">
+        <v>1812126.1325028299</v>
       </c>
       <c r="C55">
-        <v>1812126.1325028299</v>
+        <v>129993.271423178</v>
       </c>
       <c r="D55">
-        <v>129993.271423178</v>
+        <v>56556.234428085998</v>
       </c>
       <c r="E55">
-        <v>56556.234428085998</v>
+        <f t="shared" si="0"/>
+        <v>3.1209877399633868E-2</v>
       </c>
       <c r="F55">
-        <f t="shared" si="0"/>
-        <v>3.1209877399633868E-2</v>
-      </c>
-      <c r="G55">
         <f t="shared" si="1"/>
         <v>7.1735222560714879E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>14804670</v>
       </c>
-      <c r="B56" t="s">
-        <v>58</v>
+      <c r="B56">
+        <v>1805875.4990737301</v>
       </c>
       <c r="C56">
-        <v>1805875.4990737301</v>
+        <v>130582.009262689</v>
       </c>
       <c r="D56">
-        <v>130582.009262689</v>
+        <v>55830.075583549398</v>
       </c>
       <c r="E56">
-        <v>55830.075583549398</v>
+        <f t="shared" si="0"/>
+        <v>3.0915794367987033E-2</v>
       </c>
       <c r="F56">
-        <f t="shared" si="0"/>
-        <v>3.0915794367987033E-2</v>
-      </c>
-      <c r="G56">
         <f t="shared" si="1"/>
         <v>7.2309530379955397E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>20259914</v>
       </c>
-      <c r="B57" t="s">
-        <v>59</v>
+      <c r="B57">
+        <v>1787934.6664241501</v>
       </c>
       <c r="C57">
-        <v>1787934.6664241501</v>
+        <v>129399.32048017401</v>
       </c>
       <c r="D57">
-        <v>129399.32048017401</v>
+        <v>55923.591487813697</v>
       </c>
       <c r="E57">
-        <v>55923.591487813697</v>
+        <f t="shared" si="0"/>
+        <v>3.1278319358089453E-2</v>
       </c>
       <c r="F57">
-        <f t="shared" si="0"/>
-        <v>3.1278319358089453E-2</v>
-      </c>
-      <c r="G57">
         <f t="shared" si="1"/>
         <v>7.237362914326799E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>353539995</v>
       </c>
-      <c r="B58" t="s">
-        <v>60</v>
+      <c r="B58">
+        <v>1782906.8292247199</v>
       </c>
       <c r="C58">
-        <v>1782906.8292247199</v>
+        <v>128681.552697391</v>
       </c>
       <c r="D58">
-        <v>128681.552697391</v>
+        <v>55253.463379778397</v>
       </c>
       <c r="E58">
-        <v>55253.463379778397</v>
+        <f t="shared" si="0"/>
+        <v>3.099066225676237E-2</v>
       </c>
       <c r="F58">
-        <f t="shared" si="0"/>
-        <v>3.099066225676237E-2</v>
-      </c>
-      <c r="G58">
         <f t="shared" si="1"/>
         <v>7.2175141509411886E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>38053181</v>
       </c>
-      <c r="B59" t="s">
-        <v>61</v>
+      <c r="B59">
+        <v>1765718.009477</v>
       </c>
       <c r="C59">
-        <v>1765718.009477</v>
+        <v>127489.69427869401</v>
       </c>
       <c r="D59">
-        <v>127489.69427869401</v>
+        <v>54784.1375921375</v>
       </c>
       <c r="E59">
-        <v>54784.1375921375</v>
+        <f t="shared" si="0"/>
+        <v>3.1026549708446587E-2</v>
       </c>
       <c r="F59">
-        <f t="shared" si="0"/>
-        <v>3.1026549708446587E-2</v>
-      </c>
-      <c r="G59">
         <f t="shared" si="1"/>
         <v>7.2202749020188139E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>7788379</v>
       </c>
-      <c r="B60" t="s">
-        <v>62</v>
+      <c r="B60">
+        <v>1785700.5857192101</v>
       </c>
       <c r="C60">
-        <v>1785700.5857192101</v>
+        <v>129060.285270783</v>
       </c>
       <c r="D60">
-        <v>129060.285270783</v>
+        <v>55459.587098999596</v>
       </c>
       <c r="E60">
-        <v>55459.587098999596</v>
+        <f t="shared" si="0"/>
+        <v>3.105760704931541E-2</v>
       </c>
       <c r="F60">
-        <f t="shared" si="0"/>
-        <v>3.105760704931541E-2</v>
-      </c>
-      <c r="G60">
         <f t="shared" si="1"/>
         <v>7.227431423997803E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>6272357</v>
       </c>
-      <c r="B61" t="s">
-        <v>63</v>
+      <c r="B61">
+        <v>1763422.5113597801</v>
       </c>
       <c r="C61">
-        <v>1763422.5113597801</v>
+        <v>127525.35266191899</v>
       </c>
       <c r="D61">
-        <v>127525.35266191899</v>
+        <v>54715.295354357397</v>
       </c>
       <c r="E61">
-        <v>54715.295354357397</v>
+        <f t="shared" si="0"/>
+        <v>3.102789887385881E-2</v>
       </c>
       <c r="F61">
-        <f t="shared" si="0"/>
-        <v>3.102789887385881E-2</v>
-      </c>
-      <c r="G61">
         <f t="shared" si="1"/>
         <v>7.2316958551007629E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>40966108</v>
       </c>
-      <c r="B62" t="s">
-        <v>64</v>
+      <c r="B62">
+        <v>1756924.7862620801</v>
       </c>
       <c r="C62">
-        <v>1756924.7862620801</v>
+        <v>127248.4018006</v>
       </c>
       <c r="D62">
-        <v>127248.4018006</v>
+        <v>54333.613871290399</v>
       </c>
       <c r="E62">
-        <v>54333.613871290399</v>
+        <f t="shared" si="0"/>
+        <v>3.0925406879190938E-2</v>
       </c>
       <c r="F62">
-        <f t="shared" si="0"/>
-        <v>3.0925406879190938E-2</v>
-      </c>
-      <c r="G62">
         <f t="shared" si="1"/>
         <v>7.2426778195397598E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>40427625</v>
       </c>
-      <c r="B63" t="s">
-        <v>65</v>
+      <c r="B63">
+        <v>1745603.3224007799</v>
       </c>
       <c r="C63">
-        <v>1745603.3224007799</v>
+        <v>126615.81666120001</v>
       </c>
       <c r="D63">
-        <v>126615.81666120001</v>
+        <v>54108.991144637497</v>
       </c>
       <c r="E63">
-        <v>54108.991144637497</v>
+        <f t="shared" si="0"/>
+        <v>3.0997300732803258E-2</v>
       </c>
       <c r="F63">
-        <f t="shared" si="0"/>
-        <v>3.0997300732803258E-2</v>
-      </c>
-      <c r="G63">
         <f t="shared" si="1"/>
         <v>7.2534129052333335E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>82174834</v>
       </c>
-      <c r="B64" t="s">
-        <v>66</v>
+      <c r="B64">
+        <v>1744459.5680104799</v>
       </c>
       <c r="C64">
-        <v>1744459.5680104799</v>
+        <v>126532.82628646299</v>
       </c>
       <c r="D64">
-        <v>126532.82628646299</v>
+        <v>54073.523762700701</v>
       </c>
       <c r="E64">
-        <v>54073.523762700701</v>
+        <f t="shared" si="0"/>
+        <v>3.0997292659737843E-2</v>
       </c>
       <c r="F64">
-        <f t="shared" si="0"/>
-        <v>3.0997292659737843E-2</v>
-      </c>
-      <c r="G64">
         <f t="shared" si="1"/>
         <v>7.2534112344473003E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>476704454</v>
       </c>
-      <c r="B65" t="s">
-        <v>67</v>
+      <c r="B65">
+        <v>1738992.7229925799</v>
       </c>
       <c r="C65">
-        <v>1738992.7229925799</v>
+        <v>126068.051273782</v>
       </c>
       <c r="D65">
-        <v>126068.051273782</v>
+        <v>53629.105772331503</v>
       </c>
       <c r="E65">
-        <v>53629.105772331503</v>
+        <f t="shared" si="0"/>
+        <v>3.0839177797157655E-2</v>
       </c>
       <c r="F65">
-        <f t="shared" si="0"/>
-        <v>3.0839177797157655E-2</v>
-      </c>
-      <c r="G65">
         <f t="shared" si="1"/>
         <v>7.2494869936451087E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>927587</v>
       </c>
-      <c r="B66" t="s">
-        <v>68</v>
+      <c r="B66">
+        <v>1738864.9419231899</v>
       </c>
       <c r="C66">
-        <v>1738864.9419231899</v>
+        <v>126417.502697556</v>
       </c>
       <c r="D66">
-        <v>126417.502697556</v>
+        <v>54400.701364646098</v>
       </c>
       <c r="E66">
-        <v>54400.701364646098</v>
+        <f t="shared" si="0"/>
+        <v>3.1285179229893934E-2</v>
       </c>
       <c r="F66">
-        <f t="shared" si="0"/>
-        <v>3.1285179229893934E-2</v>
-      </c>
-      <c r="G66">
         <f t="shared" si="1"/>
         <v>7.2701162493814989E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>546195</v>
       </c>
-      <c r="B67" t="s">
-        <v>69</v>
+      <c r="B67">
+        <v>1787757.5523273901</v>
       </c>
       <c r="C67">
-        <v>1787757.5523273901</v>
+        <v>131420.05623242701</v>
       </c>
       <c r="D67">
-        <v>131420.05623242701</v>
+        <v>56249.695095282703</v>
       </c>
       <c r="E67">
-        <v>56249.695095282703</v>
+        <f t="shared" ref="E67:E105" si="2">D67/B67</f>
+        <v>3.1463827420029136E-2</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F105" si="2">E67/C67</f>
-        <v>3.1463827420029136E-2</v>
-      </c>
-      <c r="G67">
-        <f t="shared" ref="G67:G105" si="3">D67/C67</f>
+        <f t="shared" ref="F67:F105" si="3">C67/B67</f>
         <v>7.351111791491971E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2920960</v>
       </c>
-      <c r="B68" t="s">
-        <v>70</v>
+      <c r="B68">
+        <v>1774745.12703783</v>
       </c>
       <c r="C68">
-        <v>1774745.12703783</v>
+        <v>130326.887419255</v>
       </c>
       <c r="D68">
-        <v>130326.887419255</v>
+        <v>55557.6102737619</v>
       </c>
       <c r="E68">
-        <v>55557.6102737619</v>
+        <f t="shared" si="2"/>
+        <v>3.1304557159985737E-2</v>
       </c>
       <c r="F68">
-        <f t="shared" si="2"/>
-        <v>3.1304557159985737E-2</v>
-      </c>
-      <c r="G68">
         <f t="shared" si="3"/>
         <v>7.3434142984113673E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>13164144</v>
       </c>
-      <c r="B69" t="s">
-        <v>71</v>
+      <c r="B69">
+        <v>1764521.28779157</v>
       </c>
       <c r="C69">
-        <v>1764521.28779157</v>
+        <v>129356.30566495001</v>
       </c>
       <c r="D69">
-        <v>129356.30566495001</v>
+        <v>55084.199333535202</v>
       </c>
       <c r="E69">
-        <v>55084.199333535202</v>
+        <f t="shared" si="2"/>
+        <v>3.1217645099922364E-2</v>
       </c>
       <c r="F69">
-        <f t="shared" si="2"/>
-        <v>3.1217645099922364E-2</v>
-      </c>
-      <c r="G69">
         <f t="shared" si="3"/>
         <v>7.3309574987813875E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>396806711</v>
       </c>
-      <c r="B70" t="s">
-        <v>72</v>
+      <c r="B70">
+        <v>1748434.00417785</v>
       </c>
       <c r="C70">
-        <v>1748434.00417785</v>
+        <v>128036.791703968</v>
       </c>
       <c r="D70">
-        <v>128036.791703968</v>
+        <v>54399.799761265203</v>
       </c>
       <c r="E70">
-        <v>54399.799761265203</v>
+        <f t="shared" si="2"/>
+        <v>3.1113441875002378E-2</v>
       </c>
       <c r="F70">
-        <f t="shared" si="2"/>
-        <v>3.1113441875002378E-2</v>
-      </c>
-      <c r="G70">
         <f t="shared" si="3"/>
         <v>7.3229410660068675E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>158119101</v>
       </c>
-      <c r="B71" t="s">
-        <v>73</v>
+      <c r="B71">
+        <v>1748296.85416054</v>
       </c>
       <c r="C71">
-        <v>1748296.85416054</v>
+        <v>128059.906204057</v>
       </c>
       <c r="D71">
-        <v>128059.906204057</v>
+        <v>54753.062040576297</v>
       </c>
       <c r="E71">
-        <v>54753.062040576297</v>
+        <f t="shared" si="2"/>
+        <v>3.1317943466109166E-2</v>
       </c>
       <c r="F71">
-        <f t="shared" si="2"/>
-        <v>3.1317943466109166E-2</v>
-      </c>
-      <c r="G71">
         <f t="shared" si="3"/>
         <v>7.3248376498135426E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>249115678</v>
       </c>
-      <c r="B72" t="s">
-        <v>74</v>
+      <c r="B72">
+        <v>1743362.7615183999</v>
       </c>
       <c r="C72">
-        <v>1743362.7615183999</v>
+        <v>127081.031874818</v>
       </c>
       <c r="D72">
-        <v>127081.031874818</v>
+        <v>54106.998261373497</v>
       </c>
       <c r="E72">
-        <v>54106.998261373497</v>
+        <f t="shared" si="2"/>
+        <v>3.1035995178793681E-2</v>
       </c>
       <c r="F72">
-        <f t="shared" si="2"/>
-        <v>3.1035995178793681E-2</v>
-      </c>
-      <c r="G72">
         <f t="shared" si="3"/>
         <v>7.2894198889584774E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1420982</v>
       </c>
-      <c r="B73" t="s">
-        <v>75</v>
+      <c r="B73">
+        <v>1763588.1382462101</v>
       </c>
       <c r="C73">
-        <v>1763588.1382462101</v>
+        <v>128895.50271351</v>
       </c>
       <c r="D73">
-        <v>128895.50271351</v>
+        <v>54760.760354184502</v>
       </c>
       <c r="E73">
-        <v>54760.760354184502</v>
+        <f t="shared" si="2"/>
+        <v>3.1050764725964318E-2</v>
       </c>
       <c r="F73">
-        <f t="shared" si="2"/>
-        <v>3.1050764725964318E-2</v>
-      </c>
-      <c r="G73">
         <f t="shared" si="3"/>
         <v>7.3087077372662179E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>477531206</v>
       </c>
-      <c r="B74" t="s">
-        <v>76</v>
+      <c r="B74">
+        <v>1758751.4967614701</v>
       </c>
       <c r="C74">
-        <v>1758751.4967614701</v>
+        <v>128335.191776964</v>
       </c>
       <c r="D74">
-        <v>128335.191776964</v>
+        <v>54083.669670515301</v>
       </c>
       <c r="E74">
-        <v>54083.669670515301</v>
+        <f t="shared" si="2"/>
+        <v>3.075117193651513E-2</v>
       </c>
       <c r="F74">
-        <f t="shared" si="2"/>
-        <v>3.075117193651513E-2</v>
-      </c>
-      <c r="G74">
         <f t="shared" si="3"/>
         <v>7.2969485463567685E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>113362335</v>
       </c>
-      <c r="B75" t="s">
-        <v>77</v>
+      <c r="B75">
+        <v>1758860.9502915801</v>
       </c>
       <c r="C75">
-        <v>1758860.9502915801</v>
+        <v>128787.327409053</v>
       </c>
       <c r="D75">
-        <v>128787.327409053</v>
+        <v>53856.038322688102</v>
       </c>
       <c r="E75">
-        <v>53856.038322688102</v>
+        <f t="shared" si="2"/>
+        <v>3.0619838545940751E-2</v>
       </c>
       <c r="F75">
-        <f t="shared" si="2"/>
-        <v>3.0619838545940751E-2</v>
-      </c>
-      <c r="G75">
         <f t="shared" si="3"/>
         <v>7.3222006201060369E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2200736</v>
       </c>
-      <c r="B76" t="s">
-        <v>78</v>
+      <c r="B76">
+        <v>1781579.03560668</v>
       </c>
       <c r="C76">
-        <v>1781579.03560668</v>
+        <v>132471.33607230801</v>
       </c>
       <c r="D76">
-        <v>132471.33607230801</v>
+        <v>58292.532730758699</v>
       </c>
       <c r="E76">
-        <v>58292.532730758699</v>
+        <f t="shared" si="2"/>
+        <v>3.2719588390816678E-2</v>
       </c>
       <c r="F76">
-        <f t="shared" si="2"/>
-        <v>3.2719588390816678E-2</v>
-      </c>
-      <c r="G76">
         <f t="shared" si="3"/>
         <v>7.4356137687261029E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>297344797</v>
       </c>
-      <c r="B77" t="s">
-        <v>79</v>
+      <c r="B77">
+        <v>1770027.49527154</v>
       </c>
       <c r="C77">
-        <v>1770027.49527154</v>
+        <v>131767.024317751</v>
       </c>
       <c r="D77">
-        <v>131767.024317751</v>
+        <v>57895.757092677602</v>
       </c>
       <c r="E77">
-        <v>57895.757092677602</v>
+        <f t="shared" si="2"/>
+        <v>3.2708959181335096E-2</v>
       </c>
       <c r="F77">
-        <f t="shared" si="2"/>
-        <v>3.2708959181335096E-2</v>
-      </c>
-      <c r="G77">
         <f t="shared" si="3"/>
         <v>7.444349009817873E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>393166851</v>
       </c>
-      <c r="B78" t="s">
-        <v>80</v>
+      <c r="B78">
+        <v>1783474.5593175101</v>
       </c>
       <c r="C78">
-        <v>1783474.5593175101</v>
+        <v>132577.224473473</v>
       </c>
       <c r="D78">
-        <v>132577.224473473</v>
+        <v>58090.222340709101</v>
       </c>
       <c r="E78">
-        <v>58090.222340709101</v>
+        <f t="shared" si="2"/>
+        <v>3.2571377055660794E-2</v>
       </c>
       <c r="F78">
-        <f t="shared" si="2"/>
-        <v>3.2571377055660794E-2</v>
-      </c>
-      <c r="G78">
         <f t="shared" si="3"/>
         <v>7.4336481998491133E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>99157282</v>
       </c>
-      <c r="B79" t="s">
-        <v>81</v>
+      <c r="B79">
+        <v>1804647.6372007299</v>
       </c>
       <c r="C79">
-        <v>1804647.6372007299</v>
+        <v>134293.560378847</v>
       </c>
       <c r="D79">
-        <v>134293.560378847</v>
+        <v>59104.281241778401</v>
       </c>
       <c r="E79">
-        <v>59104.281241778401</v>
+        <f t="shared" si="2"/>
+        <v>3.2751147660857335E-2</v>
       </c>
       <c r="F79">
-        <f t="shared" si="2"/>
-        <v>3.2751147660857335E-2</v>
-      </c>
-      <c r="G79">
         <f t="shared" si="3"/>
         <v>7.4415391465092753E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>81824112</v>
       </c>
-      <c r="B80" t="s">
-        <v>82</v>
+      <c r="B80">
+        <v>1824614.2594131301</v>
       </c>
       <c r="C80">
-        <v>1824614.2594131301</v>
+        <v>135847.576733316</v>
       </c>
       <c r="D80">
-        <v>135847.576733316</v>
+        <v>60988.312905738698</v>
       </c>
       <c r="E80">
-        <v>60988.312905738698</v>
+        <f t="shared" si="2"/>
+        <v>3.3425318579585701E-2</v>
       </c>
       <c r="F80">
-        <f t="shared" si="2"/>
-        <v>3.3425318579585701E-2</v>
-      </c>
-      <c r="G80">
         <f t="shared" si="3"/>
         <v>7.4452765033750257E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>433351</v>
       </c>
-      <c r="B81" t="s">
-        <v>83</v>
+      <c r="B81">
+        <v>1812431.7159702601</v>
       </c>
       <c r="C81">
-        <v>1812431.7159702601</v>
+        <v>134915.6229172</v>
       </c>
       <c r="D81">
-        <v>134915.6229172</v>
+        <v>60747.432453217101</v>
       </c>
       <c r="E81">
-        <v>60747.432453217101</v>
+        <f t="shared" si="2"/>
+        <v>3.3517087522768718E-2</v>
       </c>
       <c r="F81">
-        <f t="shared" si="2"/>
-        <v>3.3517087522768718E-2</v>
-      </c>
-      <c r="G81">
         <f t="shared" si="3"/>
         <v>7.4439010158777102E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>106685726</v>
       </c>
-      <c r="B82" t="s">
-        <v>84</v>
+      <c r="B82">
+        <v>1809410.68387749</v>
       </c>
       <c r="C82">
-        <v>1809410.68387749</v>
+        <v>134839.56719817701</v>
       </c>
       <c r="D82">
-        <v>134839.56719817701</v>
+        <v>60785.258921791901</v>
       </c>
       <c r="E82">
-        <v>60785.258921791901</v>
+        <f t="shared" si="2"/>
+        <v>3.359395380131816E-2</v>
       </c>
       <c r="F82">
-        <f t="shared" si="2"/>
-        <v>3.359395380131816E-2</v>
-      </c>
-      <c r="G82">
         <f t="shared" si="3"/>
         <v>7.4521261756464022E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>28266043</v>
       </c>
-      <c r="B83" t="s">
-        <v>85</v>
+      <c r="B83">
+        <v>1800816.1977005701</v>
       </c>
       <c r="C83">
-        <v>1800816.1977005701</v>
+        <v>134033.18095476099</v>
       </c>
       <c r="D83">
-        <v>134033.18095476099</v>
+        <v>60499.209697575599</v>
       </c>
       <c r="E83">
-        <v>60499.209697575599</v>
+        <f t="shared" si="2"/>
+        <v>3.3595438432209766E-2</v>
       </c>
       <c r="F83">
-        <f t="shared" si="2"/>
-        <v>3.3595438432209766E-2</v>
-      </c>
-      <c r="G83">
         <f t="shared" si="3"/>
         <v>7.4429128928263505E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>404216060</v>
       </c>
-      <c r="B84" t="s">
-        <v>86</v>
+      <c r="B84">
+        <v>1801682.80844236</v>
       </c>
       <c r="C84">
-        <v>1801682.80844236</v>
+        <v>134655.78647247501</v>
       </c>
       <c r="D84">
-        <v>134655.78647247501</v>
+        <v>60844.654653172001</v>
       </c>
       <c r="E84">
-        <v>60844.654653172001</v>
+        <f t="shared" si="2"/>
+        <v>3.3771013614641236E-2</v>
       </c>
       <c r="F84">
-        <f t="shared" si="2"/>
-        <v>3.3771013614641236E-2</v>
-      </c>
-      <c r="G84">
         <f t="shared" si="3"/>
         <v>7.4738897347247993E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>672328094</v>
       </c>
-      <c r="B85" t="s">
-        <v>87</v>
+      <c r="B85">
+        <v>1784591.2840770499</v>
       </c>
       <c r="C85">
-        <v>1784591.2840770499</v>
+        <v>133463.77688368599</v>
       </c>
       <c r="D85">
-        <v>133463.77688368599</v>
+        <v>60304.811997073797</v>
       </c>
       <c r="E85">
-        <v>60304.811997073797</v>
+        <f t="shared" si="2"/>
+        <v>3.3791945828236004E-2</v>
       </c>
       <c r="F85">
-        <f t="shared" si="2"/>
-        <v>3.3791945828236004E-2</v>
-      </c>
-      <c r="G85">
         <f t="shared" si="3"/>
         <v>7.4786747012894006E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>313580179</v>
       </c>
-      <c r="B86" t="s">
-        <v>88</v>
+      <c r="B86">
+        <v>1781421.98530474</v>
       </c>
       <c r="C86">
-        <v>1781421.98530474</v>
+        <v>132773.58154661499</v>
       </c>
       <c r="D86">
-        <v>132773.58154661499</v>
+        <v>60007.045531197298</v>
       </c>
       <c r="E86">
-        <v>60007.045531197298</v>
+        <f t="shared" si="2"/>
+        <v>3.3684913527623359E-2</v>
       </c>
       <c r="F86">
-        <f t="shared" si="2"/>
-        <v>3.3684913527623359E-2</v>
-      </c>
-      <c r="G86">
         <f t="shared" si="3"/>
         <v>7.4532358218259001E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>347667464</v>
       </c>
-      <c r="B87" t="s">
-        <v>89</v>
+      <c r="B87">
+        <v>1779452.24517971</v>
       </c>
       <c r="C87">
-        <v>1779452.24517971</v>
+        <v>132378.46845988999</v>
       </c>
       <c r="D87">
-        <v>132378.46845988999</v>
+        <v>59941.370864079901</v>
       </c>
       <c r="E87">
-        <v>59941.370864079901</v>
+        <f t="shared" si="2"/>
+        <v>3.3685293340382012E-2</v>
       </c>
       <c r="F87">
-        <f t="shared" si="2"/>
-        <v>3.3685293340382012E-2</v>
-      </c>
-      <c r="G87">
         <f t="shared" si="3"/>
         <v>7.4392818811791633E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>7946432</v>
       </c>
-      <c r="B88" t="s">
-        <v>90</v>
+      <c r="B88">
+        <v>1762542.3674429499</v>
       </c>
       <c r="C88">
-        <v>1762542.3674429499</v>
+        <v>131080.035050576</v>
       </c>
       <c r="D88">
-        <v>131080.035050576</v>
+        <v>59306.623617972196</v>
       </c>
       <c r="E88">
-        <v>59306.623617972196</v>
+        <f t="shared" si="2"/>
+        <v>3.3648339304327014E-2</v>
       </c>
       <c r="F88">
-        <f t="shared" si="2"/>
-        <v>3.3648339304327014E-2</v>
-      </c>
-      <c r="G88">
         <f t="shared" si="3"/>
         <v>7.4369863370004244E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>18202105</v>
       </c>
-      <c r="B89" t="s">
-        <v>91</v>
+      <c r="B89">
+        <v>1820142.71750755</v>
       </c>
       <c r="C89">
-        <v>1820142.71750755</v>
+        <v>135590.22273889699</v>
       </c>
       <c r="D89">
-        <v>135590.22273889699</v>
+        <v>61703.977447105302</v>
       </c>
       <c r="E89">
-        <v>61703.977447105302</v>
+        <f t="shared" si="2"/>
+        <v>3.390062595289281E-2</v>
       </c>
       <c r="F89">
-        <f t="shared" si="2"/>
-        <v>3.390062595289281E-2</v>
-      </c>
-      <c r="G89">
         <f t="shared" si="3"/>
         <v>7.4494280824621409E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>33824345</v>
       </c>
-      <c r="B90" t="s">
-        <v>92</v>
+      <c r="B90">
+        <v>1838726.72695931</v>
       </c>
       <c r="C90">
-        <v>1838726.72695931</v>
+        <v>136447.527235118</v>
       </c>
       <c r="D90">
-        <v>136447.527235118</v>
+        <v>61715.7168467019</v>
       </c>
       <c r="E90">
-        <v>61715.7168467019</v>
+        <f t="shared" si="2"/>
+        <v>3.3564376882018118E-2</v>
       </c>
       <c r="F90">
-        <f t="shared" si="2"/>
-        <v>3.3564376882018118E-2</v>
-      </c>
-      <c r="G90">
         <f t="shared" si="3"/>
         <v>7.4207616191428488E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>59905809</v>
       </c>
-      <c r="B91" t="s">
-        <v>93</v>
+      <c r="B91">
+        <v>1843410.90433992</v>
       </c>
       <c r="C91">
-        <v>1843410.90433992</v>
+        <v>137011.49625085201</v>
       </c>
       <c r="D91">
-        <v>137011.49625085201</v>
+        <v>62062.023403771796</v>
       </c>
       <c r="E91">
-        <v>62062.023403771796</v>
+        <f t="shared" si="2"/>
+        <v>3.3666950356895431E-2</v>
       </c>
       <c r="F91">
-        <f t="shared" si="2"/>
-        <v>3.3666950356895431E-2</v>
-      </c>
-      <c r="G91">
         <f t="shared" si="3"/>
         <v>7.4324989576815187E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>515993</v>
       </c>
-      <c r="B92" t="s">
-        <v>94</v>
+      <c r="B92">
+        <v>1842165.56571556</v>
       </c>
       <c r="C92">
-        <v>1842165.56571556</v>
+        <v>137370.815771736</v>
       </c>
       <c r="D92">
-        <v>137370.815771736</v>
+        <v>61827.517636486104</v>
       </c>
       <c r="E92">
-        <v>61827.517636486104</v>
+        <f t="shared" si="2"/>
+        <v>3.356241088594563E-2</v>
       </c>
       <c r="F92">
-        <f t="shared" si="2"/>
-        <v>3.356241088594563E-2</v>
-      </c>
-      <c r="G92">
         <f t="shared" si="3"/>
         <v>7.4570287453167378E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>437957199</v>
       </c>
-      <c r="B93" t="s">
-        <v>95</v>
+      <c r="B93">
+        <v>1831106.01734875</v>
       </c>
       <c r="C93">
-        <v>1831106.01734875</v>
+        <v>136570.1227758</v>
       </c>
       <c r="D93">
-        <v>136570.1227758</v>
+        <v>61758.089857651197</v>
       </c>
       <c r="E93">
-        <v>61758.089857651197</v>
+        <f t="shared" si="2"/>
+        <v>3.3727206001469237E-2</v>
       </c>
       <c r="F93">
-        <f t="shared" si="2"/>
-        <v>3.3727206001469237E-2</v>
-      </c>
-      <c r="G93">
         <f t="shared" si="3"/>
         <v>7.4583405593052043E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>1531707</v>
       </c>
-      <c r="B94" t="s">
-        <v>96</v>
+      <c r="B94">
+        <v>1818421.0303563499</v>
       </c>
       <c r="C94">
-        <v>1818421.0303563499</v>
+        <v>135535.08205015399</v>
       </c>
       <c r="D94">
-        <v>135535.08205015399</v>
+        <v>61252.185657720998</v>
       </c>
       <c r="E94">
-        <v>61252.185657720998</v>
+        <f t="shared" si="2"/>
+        <v>3.3684270383585263E-2</v>
       </c>
       <c r="F94">
-        <f t="shared" si="2"/>
-        <v>3.3684270383585263E-2</v>
-      </c>
-      <c r="G94">
         <f t="shared" si="3"/>
         <v>7.4534488871146429E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>176037767</v>
       </c>
-      <c r="B95" t="s">
-        <v>97</v>
+      <c r="B95">
+        <v>1826915.0091383799</v>
       </c>
       <c r="C95">
-        <v>1826915.0091383799</v>
+        <v>136239.17536988601</v>
       </c>
       <c r="D95">
-        <v>136239.17536988601</v>
+        <v>60999.275021758003</v>
       </c>
       <c r="E95">
-        <v>60999.275021758003</v>
+        <f t="shared" si="2"/>
+        <v>3.338922430251795E-2</v>
       </c>
       <c r="F95">
-        <f t="shared" si="2"/>
-        <v>3.338922430251795E-2</v>
-      </c>
-      <c r="G95">
         <f t="shared" si="3"/>
         <v>7.4573351627419113E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>5970160</v>
       </c>
-      <c r="B96" t="s">
-        <v>98</v>
+      <c r="B96">
+        <v>1928398.9313387801</v>
       </c>
       <c r="C96">
-        <v>1928398.9313387801</v>
+        <v>141313.275290572</v>
       </c>
       <c r="D96">
-        <v>141313.275290572</v>
+        <v>62825.642703400699</v>
       </c>
       <c r="E96">
-        <v>62825.642703400699</v>
+        <f t="shared" si="2"/>
+        <v>3.2579173158836149E-2</v>
       </c>
       <c r="F96">
-        <f t="shared" si="2"/>
-        <v>3.2579173158836149E-2</v>
-      </c>
-      <c r="G96">
         <f t="shared" si="3"/>
         <v>7.3280104543755401E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>192090</v>
       </c>
-      <c r="B97" t="s">
-        <v>99</v>
+      <c r="B97">
+        <v>1932135.7229557</v>
       </c>
       <c r="C97">
-        <v>1932135.7229557</v>
+        <v>141265.28407155001</v>
       </c>
       <c r="D97">
-        <v>141265.28407155001</v>
+        <v>62878.8330494037</v>
       </c>
       <c r="E97">
-        <v>62878.8330494037</v>
+        <f t="shared" si="2"/>
+        <v>3.2543693645503489E-2</v>
       </c>
       <c r="F97">
-        <f t="shared" si="2"/>
-        <v>3.2543693645503489E-2</v>
-      </c>
-      <c r="G97">
         <f t="shared" si="3"/>
         <v>7.311354083110079E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>23947287</v>
       </c>
-      <c r="B98" t="s">
-        <v>100</v>
+      <c r="B98">
+        <v>1963306.5141171501</v>
       </c>
       <c r="C98">
-        <v>1963306.5141171501</v>
+        <v>142661.467340918</v>
       </c>
       <c r="D98">
-        <v>142661.467340918</v>
+        <v>63528.746312684299</v>
       </c>
       <c r="E98">
-        <v>63528.746312684299</v>
+        <f t="shared" si="2"/>
+        <v>3.2358037757161721E-2</v>
       </c>
       <c r="F98">
-        <f t="shared" si="2"/>
-        <v>3.2358037757161721E-2</v>
-      </c>
-      <c r="G98">
         <f t="shared" si="3"/>
         <v>7.2663879182955443E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>355596637</v>
       </c>
-      <c r="B99" t="s">
-        <v>101</v>
+      <c r="B99">
+        <v>1953441.5239783099</v>
       </c>
       <c r="C99">
-        <v>1953441.5239783099</v>
+        <v>141687.173686405</v>
       </c>
       <c r="D99">
-        <v>141687.173686405</v>
+        <v>63001.897414512001</v>
       </c>
       <c r="E99">
-        <v>63001.897414512001</v>
+        <f t="shared" si="2"/>
+        <v>3.2251744749545695E-2</v>
       </c>
       <c r="F99">
-        <f t="shared" si="2"/>
-        <v>3.2251744749545695E-2</v>
-      </c>
-      <c r="G99">
         <f t="shared" si="3"/>
         <v>7.2532078358736804E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>946974</v>
       </c>
-      <c r="B100" t="s">
-        <v>102</v>
+      <c r="B100">
+        <v>1945131.76104003</v>
       </c>
       <c r="C100">
-        <v>1945131.76104003</v>
+        <v>141227.23937267801</v>
       </c>
       <c r="D100">
-        <v>141227.23937267801</v>
+        <v>62730.909409822503</v>
       </c>
       <c r="E100">
-        <v>62730.909409822503</v>
+        <f t="shared" si="2"/>
+        <v>3.2250210842416818E-2</v>
       </c>
       <c r="F100">
-        <f t="shared" si="2"/>
-        <v>3.2250210842416818E-2</v>
-      </c>
-      <c r="G100">
         <f t="shared" si="3"/>
         <v>7.2605487299824939E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>20165629</v>
       </c>
-      <c r="B101" t="s">
-        <v>103</v>
+      <c r="B101">
+        <v>1927547.53145424</v>
       </c>
       <c r="C101">
-        <v>1927547.53145424</v>
+        <v>140076.45690359399</v>
       </c>
       <c r="D101">
-        <v>140076.45690359399</v>
+        <v>62117.538398692799</v>
       </c>
       <c r="E101">
-        <v>62117.538398692799</v>
+        <f t="shared" si="2"/>
+        <v>3.2226203185676136E-2</v>
       </c>
       <c r="F101">
-        <f t="shared" si="2"/>
-        <v>3.2226203185676136E-2</v>
-      </c>
-      <c r="G101">
         <f t="shared" si="3"/>
         <v>7.2670818549368368E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>416128940</v>
       </c>
-      <c r="B102" t="s">
-        <v>104</v>
+      <c r="B102">
+        <v>1932731.2072381701</v>
       </c>
       <c r="C102">
-        <v>1932731.2072381701</v>
+        <v>140760.86938940501</v>
       </c>
       <c r="D102">
-        <v>140760.86938940501</v>
+        <v>62289.901334411603</v>
       </c>
       <c r="E102">
-        <v>62289.901334411603</v>
+        <f t="shared" si="2"/>
+        <v>3.2228952014192645E-2</v>
       </c>
       <c r="F102">
-        <f t="shared" si="2"/>
-        <v>3.2228952014192645E-2</v>
-      </c>
-      <c r="G102">
         <f t="shared" si="3"/>
         <v>7.283002875011739E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>147166910</v>
       </c>
-      <c r="B103" t="s">
-        <v>105</v>
+      <c r="B103">
+        <v>1938147.62369895</v>
       </c>
       <c r="C103">
-        <v>1938147.62369895</v>
+        <v>141666.05724579599</v>
       </c>
       <c r="D103">
-        <v>141666.05724579599</v>
+        <v>62424.441953562797</v>
       </c>
       <c r="E103">
-        <v>62424.441953562797</v>
+        <f t="shared" si="2"/>
+        <v>3.2208300952032691E-2</v>
       </c>
       <c r="F103">
-        <f t="shared" si="2"/>
-        <v>3.2208300952032691E-2</v>
-      </c>
-      <c r="G103">
         <f t="shared" si="3"/>
         <v>7.3093532976309966E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>19642758</v>
       </c>
-      <c r="B104" t="s">
-        <v>106</v>
+      <c r="B104">
+        <v>1951170.17419738</v>
       </c>
       <c r="C104">
-        <v>1951170.17419738</v>
+        <v>143241.03983353099</v>
       </c>
       <c r="D104">
-        <v>143241.03983353099</v>
+        <v>63163.3648434403</v>
       </c>
       <c r="E104">
-        <v>63163.3648434403</v>
+        <f t="shared" si="2"/>
+        <v>3.2372043032803506E-2</v>
       </c>
       <c r="F104">
-        <f t="shared" si="2"/>
-        <v>3.2372043032803506E-2</v>
-      </c>
-      <c r="G104">
         <f t="shared" si="3"/>
         <v>7.3412889212727761E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>13354765</v>
       </c>
-      <c r="B105" t="s">
-        <v>107</v>
+      <c r="B105">
+        <v>1968197.45467032</v>
       </c>
       <c r="C105">
-        <v>1968197.45467032</v>
+        <v>144619.34615384601</v>
       </c>
       <c r="D105">
-        <v>144619.34615384601</v>
+        <v>63545.9807692307</v>
       </c>
       <c r="E105">
-        <v>63545.9807692307</v>
+        <f t="shared" si="2"/>
+        <v>3.2286384995795496E-2</v>
       </c>
       <c r="F105">
-        <f t="shared" si="2"/>
-        <v>3.2286384995795496E-2</v>
-      </c>
-      <c r="G105">
         <f t="shared" si="3"/>
         <v>7.3478067868993482E-2</v>
       </c>

</xml_diff>